<commit_message>
update total estimate work search in EstimateReader
</commit_message>
<xml_diff>
--- a/POSCoreTests/EstimateLogic/EstimateReaderTestsPackage/defaultEstimateWorkSheet0.xlsx
+++ b/POSCoreTests/EstimateLogic/EstimateReaderTestsPackage/defaultEstimateWorkSheet0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kss\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kss\source\repos\POS\POSCoreTests\EstimateLogic\EstimateReaderTestsPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E056371-DF9D-4109-B3D0-4CE639DC5B5B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830E8818-1B35-4C57-AFDC-71A3EBEC5518}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="48" windowWidth="19032" windowHeight="11508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="196">
   <si>
     <t>НАИМЕНОВАНИЕ УТВЕРЖДАЮЩЕЙ ОРГАНИЗАЦИИ</t>
   </si>
@@ -657,9 +657,6 @@
   </si>
   <si>
     <t>ВОЗВРАТНЫЕ СУММЫ</t>
-  </si>
-  <si>
-    <t>ПОДПУНКТ 34.1 ИНСТРУКЦИИ</t>
   </si>
   <si>
     <t>ВСЕГО ПО СВОДНОМУ СМЕТНОМУ РАСЧЕТУ</t>
@@ -898,22 +895,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -952,6 +934,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1313,13 +1310,13 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1377,13 +1374,13 @@
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -1397,45 +1394,45 @@
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:48" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1458,32 +1455,32 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="19" t="s">
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="19" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -1498,15 +1495,15 @@
       <c r="G23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="6" t="s">
         <v>29</v>
       </c>
@@ -1519,7 +1516,7 @@
       <c r="G24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="20"/>
+      <c r="H24" s="15"/>
       <c r="I24" s="6" t="s">
         <v>37</v>
       </c>
@@ -1555,16 +1552,16 @@
     </row>
     <row r="26" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -1600,7 +1597,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>41</v>
@@ -1682,16 +1679,16 @@
     </row>
     <row r="31" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -1751,16 +1748,16 @@
     </row>
     <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -1847,16 +1844,16 @@
     </row>
     <row r="38" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
     </row>
     <row r="39" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -1933,16 +1930,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -2045,16 +2042,16 @@
     </row>
     <row r="48" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
@@ -2087,23 +2084,23 @@
     </row>
     <row r="50" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>41</v>
@@ -2285,16 +2282,16 @@
     </row>
     <row r="58" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
@@ -2791,10 +2788,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>184</v>
-      </c>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
       <c r="B78" s="11" t="s">
         <v>183</v>
       </c>
@@ -2811,7 +2806,7 @@
     <row r="79" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>154</v>
@@ -2860,31 +2855,31 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="H82" s="14"/>
+      <c r="G82" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="H82" s="29"/>
       <c r="I82" s="3"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
-      <c r="C83" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D83" s="16"/>
+      <c r="C83" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" s="31"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
-      <c r="G83" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="H83" s="16"/>
+      <c r="G83" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="H83" s="31"/>
       <c r="I83" s="3"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -2901,31 +2896,31 @@
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="H85" s="14"/>
+      <c r="G85" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="H85" s="29"/>
       <c r="I85" s="3"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
-      <c r="C86" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D86" s="16"/>
+      <c r="C86" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="31"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="H86" s="16"/>
+      <c r="G86" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="H86" s="31"/>
       <c r="I86" s="3"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -2942,31 +2937,31 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H88" s="14"/>
+      <c r="G88" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="H88" s="29"/>
       <c r="I88" s="3"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
-      <c r="C89" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D89" s="16"/>
+      <c r="C89" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D89" s="31"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="H89" s="16"/>
+      <c r="G89" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="H89" s="31"/>
       <c r="I89" s="3"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -12585,6 +12580,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B38:I38"/>
     <mergeCell ref="B34:I34"/>
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="I22:I23"/>
@@ -12599,20 +12608,6 @@
     <mergeCell ref="C22:H22"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="H23:H24"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G82:H82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="G86:H86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="93" orientation="landscape" r:id="rId1"/>

</xml_diff>